<commit_message>
Tuning for paper only for -3 Month
</commit_message>
<xml_diff>
--- a/Data_Learning_Prediction/FeatureSelection_CHN_GBR_841810_same_pivot.xlsx
+++ b/Data_Learning_Prediction/FeatureSelection_CHN_GBR_841810_same_pivot.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2837" uniqueCount="86">
   <si>
     <t>month</t>
   </si>
@@ -537,13 +537,13 @@
     <t>sqrt</t>
   </si>
   <si>
-    <t>Average of value</t>
-  </si>
-  <si>
     <t>Column Labels</t>
   </si>
   <si>
     <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Min of value</t>
   </si>
 </sst>
 </file>
@@ -6642,32 +6642,32 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:J27" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <location ref="B3:K8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="4">
-    <pivotField axis="axisRow" showAll="0">
+    <pivotField name="Month Combination" axis="axisRow" multipleItemSelectionAllowed="1" showAll="0">
       <items count="23">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="20"/>
-        <item x="19"/>
-        <item x="21"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
+        <item h="1" x="0"/>
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item h="1" x="20"/>
+        <item h="1" x="19"/>
+        <item h="1" x="21"/>
+        <item h="1" x="3"/>
+        <item h="1" x="4"/>
+        <item h="1" x="5"/>
         <item x="6"/>
         <item x="7"/>
         <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
+        <item h="1" x="9"/>
+        <item h="1" x="10"/>
+        <item h="1" x="11"/>
+        <item h="1" x="12"/>
+        <item h="1" x="13"/>
+        <item h="1" x="14"/>
+        <item h="1" x="15"/>
+        <item h="1" x="16"/>
+        <item h="1" x="17"/>
+        <item h="1" x="18"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6691,34 +6691,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="22">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
+  <rowItems count="3">
     <i>
       <x v="9"/>
     </i>
@@ -6727,36 +6700,6 @@
     </i>
     <i>
       <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
     </i>
   </rowItems>
   <colFields count="2">
@@ -6796,7 +6739,7 @@
     </i>
   </colItems>
   <dataFields count="1">
-    <dataField name="Average of value" fld="2" subtotal="average" baseField="0" baseItem="298621336"/>
+    <dataField name="Min of value" fld="2" subtotal="min" baseField="0" baseItem="1"/>
   </dataFields>
   <conditionalFormats count="3">
     <conditionalFormat priority="1">
@@ -27527,782 +27470,177 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:J27"/>
+  <dimension ref="B3:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32"/>
+      <selection activeCell="C6" sqref="C6:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" customWidth="1"/>
-    <col min="6" max="10" width="7" customWidth="1"/>
-    <col min="11" max="14" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" customWidth="1"/>
+    <col min="4" max="5" width="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.44140625" customWidth="1"/>
+    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6" customWidth="1"/>
+    <col min="9" max="9" width="6.21875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B3" s="3" t="s">
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B5" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" t="s">
-        <v>80</v>
-      </c>
-      <c r="H4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5">
-        <v>50</v>
-      </c>
       <c r="C5">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="E5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="F5">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>75</v>
       </c>
       <c r="H5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="I5">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="J5">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.64620000000000011</v>
+        <v>75</v>
+      </c>
+      <c r="K5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="4" t="s">
+        <v>72</v>
       </c>
       <c r="C6" s="2">
-        <v>0.65420000000000011</v>
+        <v>0.73</v>
       </c>
       <c r="D6" s="2">
-        <v>0.64820000000000011</v>
+        <v>0.70599999999999996</v>
       </c>
       <c r="E6" s="2">
-        <v>0.56779999999999997</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="F6" s="2">
-        <v>0.56200000000000006</v>
+        <v>0.64400000000000002</v>
       </c>
       <c r="G6" s="2">
-        <v>0.56420000000000003</v>
+        <v>0.622</v>
       </c>
       <c r="H6" s="2">
-        <v>0.62119999999999997</v>
+        <v>0.61099999999999999</v>
       </c>
       <c r="I6" s="2">
-        <v>0.62220000000000009</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="J6" s="2">
-        <v>0.61119999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0.67979999999999996</v>
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.65500000000000003</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B7" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C7" s="2">
-        <v>0.68320000000000003</v>
+        <v>0.72899999999999998</v>
       </c>
       <c r="D7" s="2">
-        <v>0.68320000000000003</v>
+        <v>0.69499999999999995</v>
       </c>
       <c r="E7" s="2">
-        <v>0.59800000000000009</v>
+        <v>0.69699999999999995</v>
       </c>
       <c r="F7" s="2">
-        <v>0.58819999999999995</v>
+        <v>0.65300000000000002</v>
       </c>
       <c r="G7" s="2">
-        <v>0.58819999999999995</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="H7" s="2">
-        <v>0.6482</v>
+        <v>0.61399999999999999</v>
       </c>
       <c r="I7" s="2">
-        <v>0.64439999999999997</v>
+        <v>0.68200000000000005</v>
       </c>
       <c r="J7" s="2">
-        <v>0.64039999999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0.69759999999999989</v>
+        <v>0.66300000000000003</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.65200000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C8" s="2">
-        <v>0.68520000000000003</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="D8" s="2">
-        <v>0.68779999999999997</v>
+        <v>0.67900000000000005</v>
       </c>
       <c r="E8" s="2">
-        <v>0.60519999999999996</v>
+        <v>0.68300000000000005</v>
       </c>
       <c r="F8" s="2">
-        <v>0.60539999999999994</v>
+        <v>0.66600000000000004</v>
       </c>
       <c r="G8" s="2">
-        <v>0.60160000000000002</v>
+        <v>0.61499999999999999</v>
       </c>
       <c r="H8" s="2">
-        <v>0.67059999999999997</v>
+        <v>0.59499999999999997</v>
       </c>
       <c r="I8" s="2">
-        <v>0.65480000000000005</v>
+        <v>0.69799999999999995</v>
       </c>
       <c r="J8" s="2">
-        <v>0.64539999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0.74099999999999999</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0.72220000000000006</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.71319999999999983</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.6843999999999999</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0.65820000000000001</v>
-      </c>
-      <c r="G9" s="2">
-        <v>0.65380000000000005</v>
-      </c>
-      <c r="H9" s="2">
-        <v>0.71460000000000001</v>
-      </c>
-      <c r="I9" s="2">
-        <v>0.6986</v>
-      </c>
-      <c r="J9" s="2">
-        <v>0.68640000000000012</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="2">
-        <v>0.72260000000000002</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0.71519999999999995</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.69959999999999989</v>
-      </c>
-      <c r="E10" s="2">
-        <v>0.67460000000000009</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.6492</v>
-      </c>
-      <c r="G10" s="2">
-        <v>0.63119999999999998</v>
-      </c>
-      <c r="H10" s="2">
-        <v>0.69220000000000004</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0.68899999999999983</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0.67299999999999993</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="2">
-        <v>0.71540000000000004</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0.71120000000000005</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.69259999999999988</v>
-      </c>
-      <c r="E11" s="2">
-        <v>0.66680000000000006</v>
-      </c>
-      <c r="F11" s="2">
-        <v>0.64880000000000004</v>
-      </c>
-      <c r="G11" s="2">
-        <v>0.64179999999999993</v>
-      </c>
-      <c r="H11" s="2">
-        <v>0.6976</v>
-      </c>
-      <c r="I11" s="2">
-        <v>0.68040000000000012</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0.67860000000000009</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="B12" s="2">
-        <v>0.76319999999999999</v>
-      </c>
-      <c r="C12" s="2">
-        <v>0.73960000000000004</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.72479999999999989</v>
-      </c>
-      <c r="E12" s="2">
-        <v>0.64039999999999997</v>
-      </c>
-      <c r="F12" s="2">
-        <v>0.61219999999999997</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.60739999999999994</v>
-      </c>
-      <c r="H12" s="2">
-        <v>0.68779999999999997</v>
-      </c>
-      <c r="I12" s="2">
-        <v>0.68079999999999996</v>
-      </c>
-      <c r="J12" s="2">
-        <v>0.66720000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="2">
-        <v>0.75019999999999998</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.74240000000000006</v>
-      </c>
-      <c r="D13" s="2">
-        <v>0.72739999999999994</v>
-      </c>
-      <c r="E13" s="2">
-        <v>0.66479999999999995</v>
-      </c>
-      <c r="F13" s="2">
-        <v>0.62439999999999996</v>
-      </c>
-      <c r="G13" s="2">
-        <v>0.60699999999999998</v>
-      </c>
-      <c r="H13" s="2">
-        <v>0.69040000000000001</v>
-      </c>
-      <c r="I13" s="2">
-        <v>0.68220000000000014</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0.67020000000000013</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" s="2">
-        <v>0.76740000000000008</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.75120000000000009</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0.74080000000000001</v>
-      </c>
-      <c r="E14" s="2">
-        <v>0.65959999999999996</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.63219999999999998</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.61419999999999997</v>
-      </c>
-      <c r="H14" s="2">
-        <v>0.70760000000000001</v>
-      </c>
-      <c r="I14" s="2">
-        <v>0.69219999999999993</v>
-      </c>
-      <c r="J14" s="2">
-        <v>0.68540000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="B15" s="2">
-        <v>0.73299999999999998</v>
-      </c>
-      <c r="C15" s="2">
-        <v>0.71519999999999995</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0.70519999999999994</v>
-      </c>
-      <c r="E15" s="2">
-        <v>0.6522</v>
-      </c>
-      <c r="F15" s="2">
-        <v>0.63480000000000003</v>
-      </c>
-      <c r="G15" s="2">
-        <v>0.62379999999999991</v>
-      </c>
-      <c r="H15" s="2">
-        <v>0.68659999999999999</v>
-      </c>
-      <c r="I15" s="2">
-        <v>0.68320000000000003</v>
-      </c>
-      <c r="J15" s="2">
-        <v>0.66639999999999999</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2">
-        <v>0.73360000000000003</v>
-      </c>
-      <c r="C16" s="2">
-        <v>0.71340000000000003</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0.70939999999999992</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.65959999999999996</v>
-      </c>
-      <c r="F16" s="2">
-        <v>0.64359999999999995</v>
-      </c>
-      <c r="G16" s="2">
-        <v>0.62319999999999998</v>
-      </c>
-      <c r="H16" s="2">
-        <v>0.69499999999999995</v>
-      </c>
-      <c r="I16" s="2">
-        <v>0.66980000000000006</v>
-      </c>
-      <c r="J16" s="2">
-        <v>0.67199999999999993</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" s="2">
-        <v>0.70960000000000001</v>
-      </c>
-      <c r="C17" s="2">
-        <v>0.68720000000000003</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0.69520000000000004</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.68259999999999998</v>
-      </c>
-      <c r="F17" s="2">
-        <v>0.62619999999999998</v>
-      </c>
-      <c r="G17" s="2">
-        <v>0.60160000000000002</v>
-      </c>
-      <c r="H17" s="2">
-        <v>0.70679999999999998</v>
-      </c>
-      <c r="I17" s="2">
-        <v>0.67400000000000004</v>
-      </c>
-      <c r="J17" s="2">
-        <v>0.6604000000000001</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B18" s="2">
-        <v>0.67959999999999998</v>
-      </c>
-      <c r="C18" s="2">
-        <v>0.67620000000000002</v>
-      </c>
-      <c r="D18" s="2">
-        <v>0.68379999999999996</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="F18" s="2">
-        <v>0.59659999999999991</v>
-      </c>
-      <c r="G18" s="2">
-        <v>0.60019999999999996</v>
-      </c>
-      <c r="H18" s="2">
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="I18" s="2">
-        <v>0.64</v>
-      </c>
-      <c r="J18" s="2">
-        <v>0.64019999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19" s="2">
-        <v>0.69699999999999984</v>
-      </c>
-      <c r="C19" s="2">
-        <v>0.69100000000000006</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.70119999999999993</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.64660000000000006</v>
-      </c>
-      <c r="F19" s="2">
-        <v>0.61259999999999992</v>
-      </c>
-      <c r="G19" s="2">
-        <v>0.59499999999999997</v>
-      </c>
-      <c r="H19" s="2">
-        <v>0.68280000000000007</v>
-      </c>
-      <c r="I19" s="2">
-        <v>0.66880000000000006</v>
-      </c>
-      <c r="J19" s="2">
-        <v>0.64680000000000004</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="2">
-        <v>0.72199999999999986</v>
-      </c>
-      <c r="C20" s="2">
-        <v>0.70559999999999989</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.69219999999999993</v>
-      </c>
-      <c r="E20" s="2">
-        <v>0.63279999999999992</v>
-      </c>
-      <c r="F20" s="2">
-        <v>0.60040000000000004</v>
-      </c>
-      <c r="G20" s="2">
-        <v>0.5978</v>
-      </c>
-      <c r="H20" s="2">
-        <v>0.7006</v>
-      </c>
-      <c r="I20" s="2">
-        <v>0.66520000000000001</v>
-      </c>
-      <c r="J20" s="2">
-        <v>0.65159999999999996</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="B21" s="2">
-        <v>0.58900000000000008</v>
-      </c>
-      <c r="C21" s="2">
-        <v>0.628</v>
-      </c>
-      <c r="D21" s="2">
-        <v>0.63680000000000003</v>
-      </c>
-      <c r="E21" s="2">
-        <v>0.65380000000000016</v>
-      </c>
-      <c r="F21" s="2">
-        <v>0.58379999999999999</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0.57440000000000002</v>
-      </c>
-      <c r="H21" s="2">
-        <v>0.63939999999999997</v>
-      </c>
-      <c r="I21" s="2">
-        <v>0.63080000000000003</v>
-      </c>
-      <c r="J21" s="2">
-        <v>0.627</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="2">
-        <v>0.65159999999999996</v>
-      </c>
-      <c r="C22" s="2">
-        <v>0.6571999999999999</v>
-      </c>
-      <c r="D22" s="2">
-        <v>0.62480000000000002</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.65360000000000007</v>
-      </c>
-      <c r="F22" s="2">
-        <v>0.61380000000000001</v>
-      </c>
-      <c r="G22" s="2">
-        <v>0.57820000000000005</v>
-      </c>
-      <c r="H22" s="2">
-        <v>0.65539999999999998</v>
-      </c>
-      <c r="I22" s="2">
-        <v>0.6571999999999999</v>
-      </c>
-      <c r="J22" s="2">
-        <v>0.61159999999999992</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="2">
-        <v>0.54160000000000008</v>
-      </c>
-      <c r="C23" s="2">
-        <v>0.50460000000000005</v>
-      </c>
-      <c r="D23" s="2">
-        <v>0.50639999999999996</v>
-      </c>
-      <c r="E23" s="2">
-        <v>0.52679999999999993</v>
-      </c>
-      <c r="F23" s="2">
-        <v>0.51500000000000001</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0.49260000000000004</v>
-      </c>
-      <c r="H23" s="2">
-        <v>0.53820000000000001</v>
-      </c>
-      <c r="I23" s="2">
-        <v>0.51879999999999993</v>
-      </c>
-      <c r="J23" s="2">
-        <v>0.50600000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="B24" s="2">
-        <v>0.61599999999999999</v>
-      </c>
-      <c r="C24" s="2">
-        <v>0.64039999999999997</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.61979999999999991</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.64060000000000006</v>
-      </c>
-      <c r="F24" s="2">
-        <v>0.63480000000000003</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0.59659999999999991</v>
-      </c>
-      <c r="H24" s="2">
-        <v>0.61860000000000004</v>
-      </c>
-      <c r="I24" s="2">
-        <v>0.66359999999999997</v>
-      </c>
-      <c r="J24" s="2">
-        <v>0.60719999999999996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="2">
-        <v>0.58420000000000005</v>
-      </c>
-      <c r="C25" s="2">
-        <v>0.52800000000000002</v>
-      </c>
-      <c r="D25" s="2">
-        <v>0.52379999999999993</v>
-      </c>
-      <c r="E25" s="2">
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="F25" s="2">
-        <v>0.51859999999999995</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.52360000000000007</v>
-      </c>
-      <c r="H25" s="2">
-        <v>0.56120000000000003</v>
-      </c>
-      <c r="I25" s="2">
-        <v>0.52600000000000002</v>
-      </c>
-      <c r="J25" s="2">
-        <v>0.51340000000000008</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B26" s="2">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="C26" s="2">
-        <v>0.58899999999999997</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0.56979999999999997</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.59119999999999995</v>
-      </c>
-      <c r="F26" s="2">
-        <v>0.55579999999999996</v>
-      </c>
-      <c r="G26" s="2">
-        <v>0.55179999999999996</v>
-      </c>
-      <c r="H26" s="2">
-        <v>0.61480000000000001</v>
-      </c>
-      <c r="I26" s="2">
-        <v>0.59319999999999995</v>
-      </c>
-      <c r="J26" s="2">
-        <v>0.56879999999999997</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B27" s="2">
-        <v>0.63060000000000005</v>
-      </c>
-      <c r="C27" s="2">
-        <v>0.64319999999999999</v>
-      </c>
-      <c r="D27" s="2">
-        <v>0.64680000000000004</v>
-      </c>
-      <c r="E27" s="2">
-        <v>0.54660000000000009</v>
-      </c>
-      <c r="F27" s="2">
-        <v>0.56140000000000012</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0.5544</v>
-      </c>
-      <c r="H27" s="2">
-        <v>0.59319999999999995</v>
-      </c>
-      <c r="I27" s="2">
-        <v>0.61080000000000001</v>
-      </c>
-      <c r="J27" s="2">
-        <v>0.60539999999999983</v>
+        <v>0.65300000000000002</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.64200000000000002</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting pivot="1" sqref="B6:J27">
+  <conditionalFormatting pivot="1" sqref="C6:K8">
     <cfRule type="top10" dxfId="0" priority="3" percent="1" rank="10"/>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="B6:J27">
+  <conditionalFormatting pivot="1" sqref="C6:K8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -28312,7 +27650,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="B6:J27">
+  <conditionalFormatting pivot="1" sqref="C6:K8">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
@@ -28325,5 +27663,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>